<commit_message>
Studiumsplan Drahtlose kommunikationstechnik gestrichen und wechsel zu mobile computing angefragt
</commit_message>
<xml_diff>
--- a/Studiumplan.xlsx
+++ b/Studiumplan.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+  <workbookPr showObjects="none" codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_Programme_RB\DHBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08E1988-540C-41E8-8601-F7FA9A444D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C016C7E5-58CA-49AE-A73E-9DDC004F3A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="579" xr2:uid="{8D6EA8FC-9557-4CD3-9C64-AEC02D041DCB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="579" xr2:uid="{8D6EA8FC-9557-4CD3-9C64-AEC02D041DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Modulliste" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <author>tc={7AC76FD3-20F0-409E-BCFB-1F3017857D85}</author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{D625988B-FD12-438F-B6F9-40477B429413}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{D625988B-FD12-438F-B6F9-40477B429413}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -54,7 +54,7 @@
     wird selten angeboten</t>
       </text>
     </comment>
-    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{7AC76FD3-20F0-409E-BCFB-1F3017857D85}">
+    <comment ref="A19" authorId="1" shapeId="0" xr:uid="{7AC76FD3-20F0-409E-BCFB-1F3017857D85}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="106">
   <si>
     <t>Modulname</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Ort 2</t>
-  </si>
-  <si>
-    <t>Prüfungstermin</t>
   </si>
   <si>
     <t>MODULVERANTWORTUNG</t>
@@ -1077,18 +1074,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1104,12 +1089,258 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1134,28 +1365,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF7030A0"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1211,21 +1435,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1258,23 +1482,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1293,17 +1505,84 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <name val="Calibri Light"/>
         <family val="2"/>
         <scheme val="major"/>
@@ -1326,69 +1605,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1400,225 +1616,6 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1642,25 +1639,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1675,31 +1653,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1774,25 +1727,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F3B1065-317B-4BEC-B040-1C2152005517}" name="Modulliste" displayName="Modulliste" ref="A1:M21" totalsRowCount="1" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A1:M20" xr:uid="{4F3B1065-317B-4BEC-B040-1C2152005517}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M20">
-    <sortCondition ref="B1:B20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4F3B1065-317B-4BEC-B040-1C2152005517}" name="Modulliste" displayName="Modulliste" ref="A1:L21" totalsRowCount="1" headerRowDxfId="46" dataDxfId="45">
+  <autoFilter ref="A1:L20" xr:uid="{4F3B1065-317B-4BEC-B040-1C2152005517}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L20">
+    <sortCondition ref="C1:C20"/>
   </sortState>
-  <tableColumns count="13">
-    <tableColumn id="12" xr3:uid="{2C8AA6B6-31D0-4DF0-9DA9-0D8B08088E24}" name="Modulname" totalsRowLabel="Abschlussnote" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="1" xr3:uid="{FF50EF13-B9B2-42C9-A37F-07237C42C851}" name="Bereich" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{DE1BE470-5B26-4F88-8799-243B2BE03172}" name="Semester" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{E64020FC-6A5D-4A49-BCE1-C2569FF59159}" name="Schlüssel" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{8470E22C-4CE1-4553-8671-9BF5989AAE65}" name="Prüfungsart" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{CF2D34DC-4E44-45F0-B25E-0FFB229BA18E}" name="LP" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{80506F77-5504-411A-B364-0B22CC53A582}" name="Termin 1" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{C9413F7D-7FA1-417F-B220-3B19C8279173}" name="Ort 1" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{A89D3283-E2AE-4360-9A93-F5F27682296D}" name="Termin 2" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{DDE1A5EF-F94C-417A-95CA-A29D4C689B48}" name="Ort 2" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{A92B3274-FA6A-4C49-87BB-1CF1BAC29EAB}" name="Prüfungstermin" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{F6C0E347-9701-496F-8B92-1BFEDFF8D817}" name="MODULVERANTWORTUNG" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{A9A48352-3929-4E88-AACC-E1A6F11D63E3}" name="Note" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="21">
+  <tableColumns count="12">
+    <tableColumn id="12" xr3:uid="{2C8AA6B6-31D0-4DF0-9DA9-0D8B08088E24}" name="Modulname" totalsRowLabel="Abschlussnote" dataDxfId="44" totalsRowDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{FF50EF13-B9B2-42C9-A37F-07237C42C851}" name="Bereich" dataDxfId="43" totalsRowDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{DE1BE470-5B26-4F88-8799-243B2BE03172}" name="Semester" dataDxfId="42" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{E64020FC-6A5D-4A49-BCE1-C2569FF59159}" name="Schlüssel" dataDxfId="41" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{8470E22C-4CE1-4553-8671-9BF5989AAE65}" name="Prüfungsart" dataDxfId="40" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{CF2D34DC-4E44-45F0-B25E-0FFB229BA18E}" name="LP" dataDxfId="39" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{80506F77-5504-411A-B364-0B22CC53A582}" name="Termin 1" dataDxfId="38" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{C9413F7D-7FA1-417F-B220-3B19C8279173}" name="Ort 1" dataDxfId="37" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{A89D3283-E2AE-4360-9A93-F5F27682296D}" name="Termin 2" dataDxfId="36" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{DDE1A5EF-F94C-417A-95CA-A29D4C689B48}" name="Ort 2" dataDxfId="35" totalsRowDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{F6C0E347-9701-496F-8B92-1BFEDFF8D817}" name="MODULVERANTWORTUNG" dataDxfId="34" totalsRowDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{A9A48352-3929-4E88-AACC-E1A6F11D63E3}" name="Note" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="0">
       <totalsRowFormula array="1">SUMPRODUCT(IF(Modulliste[Note]&lt;&gt;"", Modulliste[Note]), Modulliste[LP]) / SUM(IF(Modulliste[Note]&lt;&gt;"", Modulliste[LP]))</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2097,10 +2049,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A9" dT="2023-04-18T07:11:20.76" personId="{00CAF5A1-3185-49EF-893A-254A033DD426}" id="{D625988B-FD12-438F-B6F9-40477B429413}">
+  <threadedComment ref="A12" dT="2023-04-18T07:11:20.76" personId="{00CAF5A1-3185-49EF-893A-254A033DD426}" id="{D625988B-FD12-438F-B6F9-40477B429413}">
     <text>wird selten angeboten</text>
   </threadedComment>
-  <threadedComment ref="A11" dT="2023-04-18T07:11:30.60" personId="{00CAF5A1-3185-49EF-893A-254A033DD426}" id="{7AC76FD3-20F0-409E-BCFB-1F3017857D85}">
+  <threadedComment ref="A19" dT="2023-04-18T07:11:30.60" personId="{00CAF5A1-3185-49EF-893A-254A033DD426}" id="{7AC76FD3-20F0-409E-BCFB-1F3017857D85}">
     <text>neues Modul</text>
   </threadedComment>
 </ThreadedComments>
@@ -2117,11 +2069,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70D999F-AAA9-4A38-8F55-9E1C84DAB455}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E10" sqref="E10"/>
+      <selection pane="topRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,13 +2088,12 @@
     <col min="8" max="8" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="24"/>
-    <col min="14" max="16384" width="11.42578125" style="2"/>
+    <col min="11" max="11" width="29.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="24"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2176,683 +2127,659 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="24" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="21" t="s">
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7">
+        <v>5</v>
+      </c>
+      <c r="G2" s="23">
+        <v>45029</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="23">
+        <v>45061</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="7">
+        <v>5</v>
+      </c>
+      <c r="G3" s="23">
+        <v>45036</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="23">
+        <v>45068</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="7">
+        <v>5</v>
+      </c>
+      <c r="G4" s="23">
+        <v>45043</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="23">
+        <v>45082</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="21">
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="7">
         <v>5</v>
       </c>
-      <c r="G2" s="22">
-        <v>45670</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" s="22">
-        <v>45701</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="29"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
+      <c r="G5" s="23">
+        <v>45120</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="23">
+        <v>45180</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="17">
-        <v>5</v>
-      </c>
-      <c r="G3" s="18">
-        <v>45299</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="18">
-        <v>45330</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="26"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="17">
-        <v>5</v>
-      </c>
-      <c r="G4" s="18">
-        <v>45400</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="18">
-        <v>45439</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" s="26"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="17">
-        <v>5</v>
-      </c>
-      <c r="G5" s="18">
-        <v>45481</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="18">
-        <v>45540</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="26"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="E6" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="F6" s="17">
         <v>5</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="26"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="G6" s="18">
+        <v>45299</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="18">
+        <v>45330</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="26">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="14">
+        <v>5</v>
+      </c>
+      <c r="G7" s="15">
+        <v>45323</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="15">
+        <v>45355</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="27">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+      <c r="G8" s="23">
+        <v>45218</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="23">
+        <v>45250</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="G9" s="23">
+        <v>45320</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="23">
+        <v>45358</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="25"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="17">
+        <v>5</v>
+      </c>
+      <c r="G10" s="18">
+        <v>45400</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="18">
+        <v>45439</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="26"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="17">
+        <v>5</v>
+      </c>
+      <c r="G11" s="18">
+        <v>45481</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="18">
+        <v>45502</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="26"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="19">
+        <v>5</v>
+      </c>
+      <c r="G12" s="20">
+        <v>45393</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="20">
+        <v>45425</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="28"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="19">
+        <v>5</v>
+      </c>
+      <c r="G13" s="20">
+        <v>45488</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="20">
+        <v>45547</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="28"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="21">
+        <v>5</v>
+      </c>
+      <c r="G14" s="22">
+        <v>45670</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="22">
+        <v>45701</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="29"/>
+    </row>
+    <row r="15" spans="1:12" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17">
+        <v>5</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="26"/>
+    </row>
+    <row r="16" spans="1:12" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17">
+        <v>10</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="26"/>
+    </row>
+    <row r="17" spans="1:12" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="14">
+        <v>5</v>
+      </c>
+      <c r="G17" s="15">
+        <v>45691</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="15">
+        <v>45729</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="1:12" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17">
+        <v>25</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="26"/>
+    </row>
+    <row r="19" spans="1:12" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17">
-        <v>10</v>
-      </c>
-      <c r="G7" s="18">
-        <v>45444</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="26"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="19">
+        <v>5</v>
+      </c>
+      <c r="G19" s="20">
+        <v>45782</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="20">
+        <v>45813</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="28"/>
+    </row>
+    <row r="20" spans="1:12" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="14">
+        <v>5</v>
+      </c>
+      <c r="G20" s="15">
+        <v>45848</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="15">
+        <v>45901</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" s="27"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
         <v>77</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17">
-        <v>25</v>
-      </c>
-      <c r="G8" s="18">
-        <v>45658</v>
-      </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="26"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="19">
-        <v>5</v>
-      </c>
-      <c r="G9" s="20">
-        <v>45393</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="20">
-        <v>45425</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="28"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="19">
-        <v>5</v>
-      </c>
-      <c r="G10" s="20">
-        <v>45488</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="20">
-        <v>45547</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="M10" s="28"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="19">
-        <v>5</v>
-      </c>
-      <c r="G11" s="20">
-        <v>45782</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="20">
-        <v>45813</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="M11" s="28"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="14">
-        <v>5</v>
-      </c>
-      <c r="G12" s="15">
-        <v>45323</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="15">
-        <v>45355</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="14">
-        <v>5</v>
-      </c>
-      <c r="G13" s="15">
-        <v>45691</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="15">
-        <v>45729</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="14">
-        <v>5</v>
-      </c>
-      <c r="G14" s="15">
-        <v>45848</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="15">
-        <v>45901</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="27"/>
-    </row>
-    <row r="15" spans="1:13" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="7">
-        <v>5</v>
-      </c>
-      <c r="G15" s="23">
-        <v>45029</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="23">
-        <v>45061</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="25"/>
-    </row>
-    <row r="16" spans="1:13" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="7">
-        <v>5</v>
-      </c>
-      <c r="G16" s="23">
-        <v>45036</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="23">
-        <v>45068</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="25"/>
-    </row>
-    <row r="17" spans="1:13" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="7">
-        <v>5</v>
-      </c>
-      <c r="G17" s="23">
-        <v>45043</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="23">
-        <v>45082</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="M17" s="25"/>
-    </row>
-    <row r="18" spans="1:13" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="82" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="7">
-        <v>5</v>
-      </c>
-      <c r="G18" s="23">
-        <v>45120</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="23">
-        <v>45180</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="23">
-        <v>45229</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" s="25"/>
-    </row>
-    <row r="19" spans="1:13" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="7">
-        <v>5</v>
-      </c>
-      <c r="G19" s="23">
-        <v>45218</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="23">
-        <v>45250</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" s="25"/>
-    </row>
-    <row r="20" spans="1:13" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="82" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="7">
-        <v>5</v>
-      </c>
-      <c r="G20" s="23">
-        <v>45320</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="23">
-        <v>45358</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M20" s="25"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
-        <v>78</v>
       </c>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
@@ -2864,49 +2791,46 @@
       <c r="I21" s="50"/>
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50" t="e" cm="1">
-        <f t="array" ref="M21">SUMPRODUCT(IF(Modulliste[Note]&lt;&gt;"", Modulliste[Note]), Modulliste[LP]) / SUM(IF(Modulliste[Note]&lt;&gt;"", Modulliste[LP]))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="50" cm="1">
+        <f t="array" ref="L21">SUMPRODUCT(IF(Modulliste[Note]&lt;&gt;"", Modulliste[Note]), Modulliste[LP]) / SUM(IF(Modulliste[Note]&lt;&gt;"", Modulliste[LP]))</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="E26"/>
       <c r="G26" s="12"/>
       <c r="H26" s="5"/>
       <c r="I26" s="12"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="E27"/>
       <c r="G27" s="12"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="E28"/>
       <c r="H28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2937,67 +2861,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="80">
+      <c r="A1" s="85">
         <v>2023</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="78" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="78" t="s">
+      <c r="F3" s="84"/>
+      <c r="G3" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="78" t="s">
+      <c r="H3" s="84"/>
+      <c r="I3" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="78" t="s">
+      <c r="J3" s="84"/>
+      <c r="K3" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="78" t="s">
+      <c r="L3" s="84"/>
+      <c r="M3" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="78" t="s">
+      <c r="N3" s="84"/>
+      <c r="O3" s="33" t="s">
         <v>85</v>
-      </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="33" t="s">
-        <v>86</v>
       </c>
       <c r="P3" s="43"/>
       <c r="Q3" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R3" s="43"/>
       <c r="S3" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T3" s="43"/>
       <c r="U3" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V3" s="43"/>
       <c r="W3" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X3" s="43"/>
       <c r="AC3" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3098,7 +3022,7 @@
         <v>45261</v>
       </c>
       <c r="AC4" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -3179,7 +3103,7 @@
         <v>45201</v>
       </c>
       <c r="T5" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U5" s="37">
         <f t="shared" si="0"/>
@@ -3198,14 +3122,14 @@
         <v>45262</v>
       </c>
       <c r="Z5" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA5" s="47">
         <f>COUNTIF(A4:X34,"U")</f>
         <v>26</v>
       </c>
       <c r="AC5" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3238,7 +3162,7 @@
         <v>45019</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" s="37">
         <f t="shared" si="0"/>
@@ -3305,14 +3229,14 @@
         <v>45263</v>
       </c>
       <c r="Z6" s="48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA6" s="49">
         <f>30-AA5</f>
         <v>4</v>
       </c>
       <c r="AC6" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3345,7 +3269,7 @@
         <v>45020</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I7" s="37">
         <f t="shared" si="0"/>
@@ -3392,7 +3316,7 @@
         <v>45203</v>
       </c>
       <c r="T7" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U7" s="37">
         <f t="shared" si="0"/>
@@ -3411,7 +3335,7 @@
         <v>45264</v>
       </c>
       <c r="AC7" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -3444,7 +3368,7 @@
         <v>45021</v>
       </c>
       <c r="H8" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I8" s="37">
         <f t="shared" si="0"/>
@@ -3491,7 +3415,7 @@
         <v>45204</v>
       </c>
       <c r="T8" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U8" s="37">
         <f t="shared" si="0"/>
@@ -3510,7 +3434,7 @@
         <v>45265</v>
       </c>
       <c r="AC8" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -3543,7 +3467,7 @@
         <v>45022</v>
       </c>
       <c r="H9" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I9" s="37">
         <f t="shared" si="0"/>
@@ -3590,7 +3514,7 @@
         <v>45205</v>
       </c>
       <c r="T9" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U9" s="37">
         <f t="shared" si="0"/>
@@ -3655,7 +3579,7 @@
         <v>45084</v>
       </c>
       <c r="L10" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M10" s="37">
         <f t="shared" si="0"/>
@@ -3670,7 +3594,7 @@
         <v>45145</v>
       </c>
       <c r="P10" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q10" s="37">
         <f t="shared" si="0"/>
@@ -3767,7 +3691,7 @@
         <v>45146</v>
       </c>
       <c r="P11" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q11" s="37">
         <f t="shared" si="0"/>
@@ -3848,7 +3772,7 @@
         <v>45086</v>
       </c>
       <c r="L12" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M12" s="37">
         <f t="shared" si="0"/>
@@ -3863,7 +3787,7 @@
         <v>45147</v>
       </c>
       <c r="P12" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q12" s="37">
         <f t="shared" si="0"/>
@@ -3960,7 +3884,7 @@
         <v>45148</v>
       </c>
       <c r="P13" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q13" s="37">
         <f t="shared" si="0"/>
@@ -4057,7 +3981,7 @@
         <v>45149</v>
       </c>
       <c r="P14" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q14" s="37">
         <f t="shared" si="0"/>
@@ -4350,14 +4274,14 @@
         <v>45152</v>
       </c>
       <c r="P17" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q17" s="37">
         <f t="shared" si="0"/>
         <v>45183</v>
       </c>
       <c r="R17" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S17" s="37">
         <f t="shared" si="0"/>
@@ -4446,14 +4370,14 @@
         <v>45153</v>
       </c>
       <c r="P18" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q18" s="37">
         <f t="shared" si="0"/>
         <v>45184</v>
       </c>
       <c r="R18" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S18" s="37">
         <f t="shared" si="0"/>
@@ -4542,7 +4466,7 @@
         <v>45154</v>
       </c>
       <c r="P19" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q19" s="37">
         <f t="shared" si="0"/>
@@ -4639,7 +4563,7 @@
         <v>45155</v>
       </c>
       <c r="P20" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q20" s="37">
         <f t="shared" si="0"/>
@@ -4736,7 +4660,7 @@
         <v>45156</v>
       </c>
       <c r="P21" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q21" s="37">
         <f t="shared" ref="Q21:Q34" si="9">IFERROR(IF(MONTH(Q20+1)=MONTH(Q$4),Q20+1,""),"")</f>
@@ -4809,7 +4733,7 @@
         <v>45065</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K22" s="37">
         <f t="shared" si="6"/>
@@ -5648,7 +5572,7 @@
         <v>45287</v>
       </c>
       <c r="X30" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
@@ -5745,7 +5669,7 @@
         <v>45288</v>
       </c>
       <c r="X31" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
@@ -5842,7 +5766,7 @@
         <v>45289</v>
       </c>
       <c r="X32" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
@@ -6066,17 +5990,17 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A4:X34">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="32" priority="1">
+      <formula>TODAY()=A4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>OR(A4="F",B4="F")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="30" priority="3">
       <formula>OR(A4="U",B4="U")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="29" priority="10">
       <formula>WEEKDAY(A4,2)&gt;5</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="1">
-      <formula>TODAY()=A4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -6088,8 +6012,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{2384E0C4-B432-4A69-9F1C-5FF116CB2572}">
-            <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$K$2:$K$19,A4)&gt;0))</xm:f>
+          <x14:cfRule type="expression" priority="11" id="{2384E0C4-B432-4A69-9F1C-5FF116CB2572}">
+            <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!#REF!,A4)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -6098,7 +6022,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="5" id="{01E0AAD0-3179-4A4C-A3F5-F297F1811797}">
+          <x14:cfRule type="expression" priority="12" id="{01E0AAD0-3179-4A4C-A3F5-F297F1811797}">
             <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$I$2:$I$19,A4)&gt;0,COUNTIF(Modulliste!$I$2:$I$19,A4-1)&gt;0,COUNTIF(Modulliste!$I$2:$I$19,A4-2)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
@@ -6108,7 +6032,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{732B42F6-81A6-4A60-8F1F-AD58B9AE4C14}">
+          <x14:cfRule type="expression" priority="13" id="{732B42F6-81A6-4A60-8F1F-AD58B9AE4C14}">
             <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$G$2:$G$19,A4)&gt;0,COUNTIF(Modulliste!$G$2:$G$19,A4-1)&gt;0,COUNTIF(Modulliste!$G$2:$G$19,A4-2)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
@@ -6132,7 +6056,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6144,67 +6068,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="80">
+      <c r="A1" s="85">
         <v>2024</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="78" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="78" t="s">
+      <c r="F3" s="84"/>
+      <c r="G3" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="78" t="s">
+      <c r="H3" s="84"/>
+      <c r="I3" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="78" t="s">
+      <c r="J3" s="84"/>
+      <c r="K3" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="78" t="s">
+      <c r="L3" s="84"/>
+      <c r="M3" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="78" t="s">
+      <c r="N3" s="84"/>
+      <c r="O3" s="33" t="s">
         <v>85</v>
-      </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="33" t="s">
-        <v>86</v>
       </c>
       <c r="P3" s="43"/>
       <c r="Q3" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R3" s="43"/>
       <c r="S3" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T3" s="43"/>
       <c r="U3" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V3" s="43"/>
       <c r="W3" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X3" s="43"/>
       <c r="AC3" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6253,7 +6177,7 @@
         <v>45444</v>
       </c>
       <c r="L4" s="69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M4" s="34">
         <f>DATE($A$1,7,1)</f>
@@ -6304,7 +6228,7 @@
         <v>45627</v>
       </c>
       <c r="AC4" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -6313,7 +6237,7 @@
         <v>45293</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="37">
         <f t="shared" ref="C5:C20" si="0">IFERROR(IF(MONTH(C4+1)=MONTH(C$4),C4+1,""),"")</f>
@@ -6368,7 +6292,7 @@
         <v>45506</v>
       </c>
       <c r="P5" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q5" s="37">
         <f t="shared" ref="Q5:Q9" si="6">IFERROR(IF(MONTH(Q4+1)=MONTH(Q$4),Q4+1,""),"")</f>
@@ -6403,14 +6327,14 @@
         <v>45628</v>
       </c>
       <c r="Z5" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA5" s="47">
         <f>COUNTIF(A4:X34,"U")</f>
         <v>17</v>
       </c>
       <c r="AC5" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6419,7 +6343,7 @@
         <v>45294</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="37">
         <f t="shared" si="0"/>
@@ -6450,7 +6374,7 @@
         <v>45415</v>
       </c>
       <c r="J6" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K6" s="37">
         <f t="shared" si="2"/>
@@ -6473,7 +6397,7 @@
         <v>45507</v>
       </c>
       <c r="P6" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q6" s="37">
         <f t="shared" si="6"/>
@@ -6508,14 +6432,14 @@
         <v>45629</v>
       </c>
       <c r="Z6" s="48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA6" s="49">
         <f>30-AA5</f>
         <v>13</v>
       </c>
       <c r="AC6" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -6524,7 +6448,7 @@
         <v>45295</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="0"/>
@@ -6555,7 +6479,7 @@
         <v>45416</v>
       </c>
       <c r="J7" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K7" s="37">
         <f t="shared" si="2"/>
@@ -6614,7 +6538,7 @@
         <v>45630</v>
       </c>
       <c r="AC7" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -6623,7 +6547,7 @@
         <v>45296</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="37">
         <f t="shared" si="0"/>
@@ -6646,7 +6570,7 @@
         <v>45387</v>
       </c>
       <c r="H8" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="37">
         <f t="shared" si="2"/>
@@ -6669,7 +6593,7 @@
         <v>45478</v>
       </c>
       <c r="N8" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O8" s="37">
         <f t="shared" si="5"/>
@@ -6712,7 +6636,7 @@
         <v>45631</v>
       </c>
       <c r="AC8" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -6745,7 +6669,7 @@
         <v>45388</v>
       </c>
       <c r="H9" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I9" s="37">
         <f t="shared" si="2"/>
@@ -6768,7 +6692,7 @@
         <v>45479</v>
       </c>
       <c r="N9" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O9" s="37">
         <f t="shared" si="5"/>
@@ -6811,7 +6735,7 @@
         <v>45632</v>
       </c>
       <c r="AC9" s="64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -6860,7 +6784,7 @@
         <v>45450</v>
       </c>
       <c r="L10" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M10" s="37">
         <f t="shared" si="2"/>
@@ -6957,7 +6881,7 @@
         <v>45451</v>
       </c>
       <c r="L11" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M11" s="37">
         <f t="shared" si="2"/>
@@ -7070,7 +6994,7 @@
         <v>45513</v>
       </c>
       <c r="P12" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q12" s="37">
         <f t="shared" si="5"/>
@@ -7143,7 +7067,7 @@
         <v>45422</v>
       </c>
       <c r="J13" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K13" s="37">
         <f t="shared" si="2"/>
@@ -7166,7 +7090,7 @@
         <v>45514</v>
       </c>
       <c r="P13" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q13" s="37">
         <f t="shared" si="5"/>
@@ -7231,14 +7155,14 @@
         <v>45393</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I14" s="37">
         <f t="shared" si="2"/>
         <v>45423</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K14" s="37">
         <f t="shared" si="2"/>
@@ -7327,7 +7251,7 @@
         <v>45394</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I15" s="37">
         <f t="shared" si="2"/>
@@ -7538,7 +7462,7 @@
         <v>45457</v>
       </c>
       <c r="L17" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M17" s="37">
         <f t="shared" si="2"/>
@@ -7635,7 +7559,7 @@
         <v>45458</v>
       </c>
       <c r="L18" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M18" s="37">
         <f t="shared" si="2"/>
@@ -7748,7 +7672,7 @@
         <v>45520</v>
       </c>
       <c r="P19" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q19" s="37">
         <f t="shared" si="5"/>
@@ -7821,7 +7745,7 @@
         <v>45429</v>
       </c>
       <c r="J20" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K20" s="37">
         <f t="shared" si="2"/>
@@ -7844,7 +7768,7 @@
         <v>45521</v>
       </c>
       <c r="P20" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q20" s="37">
         <f t="shared" si="5"/>
@@ -7909,14 +7833,14 @@
         <v>45400</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I21" s="37">
         <f t="shared" ref="I21:I34" si="15">IFERROR(IF(MONTH(I20+1)=MONTH(I$4),I20+1,""),"")</f>
         <v>45430</v>
       </c>
       <c r="J21" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K21" s="37">
         <f t="shared" ref="K21:K34" si="16">IFERROR(IF(MONTH(K20+1)=MONTH(K$4),K20+1,""),"")</f>
@@ -8005,7 +7929,7 @@
         <v>45401</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I22" s="37">
         <f t="shared" si="15"/>
@@ -8028,7 +7952,7 @@
         <v>45492</v>
       </c>
       <c r="N22" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O22" s="37">
         <f t="shared" si="18"/>
@@ -8125,7 +8049,7 @@
         <v>45493</v>
       </c>
       <c r="N23" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O23" s="37">
         <f t="shared" si="18"/>
@@ -8214,7 +8138,7 @@
         <v>45464</v>
       </c>
       <c r="L24" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M24" s="37">
         <f t="shared" si="17"/>
@@ -8311,7 +8235,7 @@
         <v>45465</v>
       </c>
       <c r="L25" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M25" s="37">
         <f t="shared" si="17"/>
@@ -8424,7 +8348,7 @@
         <v>45527</v>
       </c>
       <c r="P26" s="67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q26" s="72">
         <f t="shared" si="19"/>
@@ -8455,7 +8379,7 @@
         <v>45649</v>
       </c>
       <c r="X26" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -8496,7 +8420,7 @@
         <v>45436</v>
       </c>
       <c r="J27" s="67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K27" s="58">
         <f t="shared" si="16"/>
@@ -8519,7 +8443,7 @@
         <v>45528</v>
       </c>
       <c r="P27" s="67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q27" s="74">
         <f t="shared" si="19"/>
@@ -8550,7 +8474,7 @@
         <v>45650</v>
       </c>
       <c r="X27" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
@@ -8575,7 +8499,7 @@
         <v>45376</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G28" s="37">
         <f t="shared" si="14"/>
@@ -8590,7 +8514,7 @@
         <v>45437</v>
       </c>
       <c r="J28" s="67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K28" s="60">
         <f t="shared" si="16"/>
@@ -8671,14 +8595,14 @@
         <v>45377</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G29" s="37">
         <f t="shared" si="14"/>
         <v>45408</v>
       </c>
       <c r="H29" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I29" s="37">
         <f t="shared" si="15"/>
@@ -8701,7 +8625,7 @@
         <v>45499</v>
       </c>
       <c r="N29" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O29" s="37">
         <f t="shared" si="18"/>
@@ -8766,14 +8690,14 @@
         <v>45378</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" s="37">
         <f t="shared" si="14"/>
         <v>45409</v>
       </c>
       <c r="H30" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I30" s="37">
         <f t="shared" si="15"/>
@@ -8796,7 +8720,7 @@
         <v>45500</v>
       </c>
       <c r="N30" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O30" s="37">
         <f t="shared" si="18"/>
@@ -8835,7 +8759,7 @@
         <v>45653</v>
       </c>
       <c r="X30" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8860,7 +8784,7 @@
         <v>45379</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G31" s="37">
         <f t="shared" si="14"/>
@@ -8883,7 +8807,7 @@
         <v>45471</v>
       </c>
       <c r="L31" s="70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M31" s="56">
         <f t="shared" si="17"/>
@@ -8980,7 +8904,7 @@
         <v>45472</v>
       </c>
       <c r="L32" s="71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M32" s="56">
         <f t="shared" si="17"/>
@@ -9093,7 +9017,7 @@
         <v>45534</v>
       </c>
       <c r="P33" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q33" s="37">
         <f t="shared" si="19"/>
@@ -9124,7 +9048,7 @@
         <v>45656</v>
       </c>
       <c r="X33" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -9165,7 +9089,7 @@
         <v>45443</v>
       </c>
       <c r="J34" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K34" s="40" t="str">
         <f t="shared" si="16"/>
@@ -9188,7 +9112,7 @@
         <v>45535</v>
       </c>
       <c r="P34" s="68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q34" s="40" t="str">
         <f t="shared" si="19"/>
@@ -9219,7 +9143,7 @@
         <v>45657</v>
       </c>
       <c r="X34" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
@@ -9246,16 +9170,16 @@
     <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:X34">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>TODAY()=A4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>OR(A4="F",B4="F")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="26" priority="3">
       <formula>OR(A4="U",B4="U")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>WEEKDAY(A4,2)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9266,8 +9190,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{73078553-1D85-4963-A890-B3A458106B65}">
-            <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$K$2:$K$19,A4)&gt;0))</xm:f>
+          <x14:cfRule type="expression" priority="14" id="{73078553-1D85-4963-A890-B3A458106B65}">
+            <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!#REF!,A4)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -9276,7 +9200,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="5" id="{E702FC86-B431-4ADF-BD9A-51202BB2BBFC}">
+          <x14:cfRule type="expression" priority="15" id="{E702FC86-B431-4ADF-BD9A-51202BB2BBFC}">
             <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$I$2:$I$19,A4)&gt;0,COUNTIF(Modulliste!$I$2:$I$19,A4-1)&gt;0,COUNTIF(Modulliste!$I$2:$I$19,A4-2)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
@@ -9286,7 +9210,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{4B6781FC-2909-4FB0-B0A0-88C81246C83A}">
+          <x14:cfRule type="expression" priority="16" id="{4B6781FC-2909-4FB0-B0A0-88C81246C83A}">
             <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$G$2:$G$19,A4)&gt;0,COUNTIF(Modulliste!$G$2:$G$19,A4-1)&gt;0,COUNTIF(Modulliste!$G$2:$G$19,A4-2)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
@@ -9321,67 +9245,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="80">
+      <c r="A1" s="85">
         <v>2025</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="78" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="78" t="s">
+      <c r="F3" s="84"/>
+      <c r="G3" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="78" t="s">
+      <c r="H3" s="84"/>
+      <c r="I3" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="78" t="s">
+      <c r="J3" s="84"/>
+      <c r="K3" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="78" t="s">
+      <c r="L3" s="84"/>
+      <c r="M3" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="78" t="s">
+      <c r="N3" s="84"/>
+      <c r="O3" s="54" t="s">
         <v>85</v>
-      </c>
-      <c r="N3" s="79"/>
-      <c r="O3" s="54" t="s">
-        <v>86</v>
       </c>
       <c r="P3" s="55"/>
       <c r="Q3" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R3" s="55"/>
       <c r="S3" s="54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T3" s="55"/>
       <c r="U3" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V3" s="55"/>
       <c r="W3" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X3" s="55"/>
       <c r="AC3" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -9482,7 +9406,7 @@
         <v>45992</v>
       </c>
       <c r="AC4" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -9583,14 +9507,14 @@
         <v>45993</v>
       </c>
       <c r="Z5" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA5" s="47">
         <f>COUNTIF(A4:X34,"U")</f>
         <v>0</v>
       </c>
       <c r="AC5" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -9691,14 +9615,14 @@
         <v>45994</v>
       </c>
       <c r="Z6" s="48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA6" s="49">
         <f>30-AA5</f>
         <v>30</v>
       </c>
       <c r="AC6" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -9799,7 +9723,7 @@
         <v>45995</v>
       </c>
       <c r="AC7" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -9900,7 +9824,7 @@
         <v>45996</v>
       </c>
       <c r="AC8" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
@@ -12475,16 +12399,16 @@
     <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:X34">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>TODAY()=A4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>OR(A4="F",B4="F")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>OR(A4="U",B4="U")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>WEEKDAY(A4,2)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12494,8 +12418,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{D835A6D3-5669-4DDA-85F0-3476276045A2}">
-            <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$K$2:$K$20,A4)&gt;0))</xm:f>
+          <x14:cfRule type="expression" priority="17" id="{D835A6D3-5669-4DDA-85F0-3476276045A2}">
+            <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!#REF!,A4)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -12504,7 +12428,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="5" id="{1B902BD7-7D62-48F7-9850-BE4C0D74B7B2}">
+          <x14:cfRule type="expression" priority="18" id="{1B902BD7-7D62-48F7-9850-BE4C0D74B7B2}">
             <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$I$2:$I$20,A4)&gt;0,COUNTIF(Modulliste!$I$2:$I$20,A4-1)&gt;0,COUNTIF(Modulliste!$I$2:$I$20,A4-2)&gt;0))</xm:f>
             <x14:dxf>
               <fill>
@@ -12514,7 +12438,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{2762ECD2-9773-449F-9D06-621A561034D1}">
+          <x14:cfRule type="expression" priority="19" id="{2762ECD2-9773-449F-9D06-621A561034D1}">
             <xm:f>AND(NOT(A4=""),OR(COUNTIF(Modulliste!$G$2:$G$20,A4)&gt;0,COUNTIF(Modulliste!$G$2:$G$20,A4-1)&gt;0,COUNTIF(Modulliste!$G$2:$G$20,A4-2)&gt;0))</xm:f>
             <x14:dxf>
               <fill>

</xml_diff>